<commit_message>
re-calibrated wheel module 4 updated FPGA to include watchdog V2 is probably still broken
</commit_message>
<xml_diff>
--- a/V3.0/Documentation/Pin Assignments.xlsx
+++ b/V3.0/Documentation/Pin Assignments.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="4680"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -669,7 +670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
       <selection activeCell="F96" sqref="F96"/>
     </sheetView>
   </sheetViews>

</xml_diff>